<commit_message>
now with smart generate_costs
</commit_message>
<xml_diff>
--- a/results/approved_voters=300_projects=15.xlsx
+++ b/results/approved_voters=300_projects=15.xlsx
@@ -522,13 +522,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -537,22 +537,22 @@
         <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -587,19 +587,19 @@
         <v>0</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
       <c r="K3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -607,13 +607,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -622,22 +622,22 @@
         <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
       <c r="I4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" t="b">
         <v>0</v>
@@ -657,16 +657,16 @@
         <v>18</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -678,28 +678,28 @@
         <v>0</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
       </c>
       <c r="M5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="b">
         <v>0</v>
       </c>
       <c r="P5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -716,10 +716,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -757,13 +757,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -772,22 +772,22 @@
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" t="b">
         <v>0</v>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" t="b">
         <v>0</v>
@@ -807,16 +807,16 @@
         <v>21</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -828,28 +828,28 @@
         <v>0</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
       </c>
       <c r="K8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="b">
         <v>1</v>
       </c>
       <c r="M8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="b">
         <v>0</v>
       </c>
       <c r="P8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -866,10 +866,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -925,13 +925,13 @@
         <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
@@ -957,19 +957,19 @@
         <v>0</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -977,13 +977,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -992,22 +992,22 @@
         <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
       </c>
       <c r="K12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" t="b">
         <v>0</v>
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" t="b">
         <v>0</v>
@@ -1027,13 +1027,13 @@
         <v>26</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1042,22 +1042,22 @@
         <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
       </c>
       <c r="I13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
       </c>
       <c r="L13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" t="b">
         <v>0</v>
@@ -1077,13 +1077,13 @@
         <v>27</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1092,22 +1092,22 @@
         <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
       </c>
       <c r="L14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
@@ -1127,13 +1127,13 @@
         <v>28</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1142,22 +1142,22 @@
         <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="b">
         <v>1</v>
       </c>
       <c r="L15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
@@ -1177,13 +1177,13 @@
         <v>29</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1192,22 +1192,22 @@
         <v>0</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
       <c r="K16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="b">
         <v>0</v>
@@ -1227,13 +1227,13 @@
         <v>30</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1242,22 +1242,22 @@
         <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="b">
         <v>1</v>
       </c>
       <c r="L17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
found an error, added TODO, needs fixing
</commit_message>
<xml_diff>
--- a/results/approved_voters=300_projects=15.xlsx
+++ b/results/approved_voters=300_projects=15.xlsx
@@ -527,40 +527,40 @@
         <v>1</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -570,16 +570,16 @@
         </is>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -588,16 +588,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -621,40 +621,40 @@
         <v>1</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -667,46 +667,46 @@
         <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="b">
         <v>0</v>
       </c>
       <c r="L5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="b">
         <v>1</v>
       </c>
       <c r="O5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -725,40 +725,40 @@
         <v>1</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
       </c>
       <c r="O6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -777,40 +777,40 @@
         <v>1</v>
       </c>
       <c r="E7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -823,46 +823,46 @@
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
       </c>
       <c r="L8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" t="b">
         <v>1</v>
       </c>
       <c r="O8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="b">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -984,16 +984,16 @@
         <v>1</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
       </c>
       <c r="J11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -1017,40 +1017,40 @@
         <v>1</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1078,31 +1078,31 @@
         <v>0</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
       </c>
       <c r="N13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1112,40 +1112,40 @@
         </is>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="b">
         <v>1</v>
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="P14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1164,7 +1164,7 @@
         </is>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1182,31 +1182,31 @@
         <v>0</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="b">
         <v>1</v>
       </c>
       <c r="M15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" t="b">
         <v>0</v>
       </c>
       <c r="P15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1225,40 +1225,40 @@
         <v>1</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1268,7 +1268,7 @@
         </is>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1286,31 +1286,31 @@
         <v>0</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
       </c>
       <c r="N17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>